<commit_message>
#27 add some tests for X and Y directions, add the test descriptions
</commit_message>
<xml_diff>
--- a/documentations/TestsDocumentation.xlsx
+++ b/documentations/TestsDocumentation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\Studium\ZHAW\Module\02_Semester\PM2\workspaces\intellij_workspace_pm2\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E5E662-B0B6-4C01-9F93-2B2419CA9554}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE117A4-3ACC-4CDE-93AF-46A9B4DA0F7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PositionVector" sheetId="1" r:id="rId1"/>
-    <sheet name="Car" sheetId="2" r:id="rId2"/>
-    <sheet name="Game" sheetId="3" r:id="rId3"/>
+    <sheet name="Game" sheetId="3" r:id="rId1"/>
+    <sheet name="PositionVector" sheetId="1" r:id="rId2"/>
+    <sheet name="Car" sheetId="2" r:id="rId3"/>
     <sheet name="Start" sheetId="4" r:id="rId4"/>
     <sheet name="Track" sheetId="5" r:id="rId5"/>
     <sheet name="TrackBuilder" sheetId="6" r:id="rId6"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Expected result</t>
   </si>
@@ -47,13 +47,141 @@
   </si>
   <si>
     <t>Test case</t>
+  </si>
+  <si>
+    <t>doCarTurn()</t>
+  </si>
+  <si>
+    <t>{(0,0)}</t>
+  </si>
+  <si>
+    <t>{(0,0),(1,0)}</t>
+  </si>
+  <si>
+    <t>{(0,0),(1,0),(2,0),…,(20,0)}</t>
+  </si>
+  <si>
+    <r>
+      <t>(x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>start,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>),(x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>(0,0),(0,0)</t>
+  </si>
+  <si>
+    <t>(0,0),(1,0)</t>
+  </si>
+  <si>
+    <t>(0,0),(20,0)</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>(0,0),(0,1)</t>
+  </si>
+  <si>
+    <t>(0,0),(0,20)</t>
+  </si>
+  <si>
+    <t>{(0,0),(0,1),(0,2),…,(0,20)}</t>
+  </si>
+  <si>
+    <t>{(0,0),(0,1)}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +191,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -378,11 +514,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF32F72-142A-4A55-A3DA-B7452AF59065}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -392,9 +681,10 @@
     <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -409,6 +699,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -416,25 +709,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68531675-09C4-4F5D-A891-F3DADCBB6515}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF32F72-142A-4A55-A3DA-B7452AF59065}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
@@ -494,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C85FFA-4F74-4674-924A-D9BB7181864C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>

</xml_diff>

<commit_message>
#6 add argument check for acceleration
</commit_message>
<xml_diff>
--- a/documentations/TestsDocumentation.xlsx
+++ b/documentations/TestsDocumentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\Studium\ZHAW\Module\02_Semester\PM2\workspaces\intellij_workspace_pm2\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AF8C60-0D0A-40DB-ABEC-5C6041C359F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9AF4B4-214C-4EE1-B746-B39B0986C514}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Expected result</t>
   </si>
@@ -181,6 +181,21 @@
   </si>
   <si>
     <t>(0,0)</t>
+  </si>
+  <si>
+    <t>(x,y)</t>
+  </si>
+  <si>
+    <t>two cars; active car is crashed;one car remaining</t>
+  </si>
+  <si>
+    <t>second car is the winner</t>
+  </si>
+  <si>
+    <t>invalid direction</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException</t>
   </si>
 </sst>
 </file>
@@ -521,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF32F72-142A-4A55-A3DA-B7452AF59065}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -535,6 +550,7 @@
     <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -666,18 +682,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17">
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>20</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#37 add test cases
</commit_message>
<xml_diff>
--- a/documentations/TestsDocumentation.xlsx
+++ b/documentations/TestsDocumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\Studium\ZHAW\Module\02_Semester\PM2\workspaces\intellij_workspace_pm2\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A85E536-D42B-4373-9A57-0F4B76DF3F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22ED530-6410-418A-865E-57CE9AF56B79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Expected result</t>
   </si>
@@ -186,15 +186,9 @@
     <t>(x,y)</t>
   </si>
   <si>
-    <t>two cars; active car is crashed;one car remaining</t>
-  </si>
-  <si>
     <t>second car is the winner</t>
   </si>
   <si>
-    <t>invalid direction</t>
-  </si>
-  <si>
     <t>IllegalArgumentException</t>
   </si>
   <si>
@@ -253,6 +247,86 @@
   </si>
   <si>
     <t>Overflow?</t>
+  </si>
+  <si>
+    <t>Direction.UP</t>
+  </si>
+  <si>
+    <t>car finishes line in reverse direction is not winner</t>
+  </si>
+  <si>
+    <t>car finishes line in correct direction is  winner</t>
+  </si>
+  <si>
+    <t>all car crashes one is the winner</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Car </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>will be</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> accelerated und the Car is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>current</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> car</t>
+    </r>
+  </si>
+  <si>
+    <t>acceleration = Direction.UP, carIndex = FIRST_TURN_CAR_INDEX</t>
+  </si>
+  <si>
+    <t>Config.MAX cars total; All cars except one car are crashed ; the last remaining is the winner;</t>
+  </si>
+  <si>
+    <t>Two cars, crash one, the last is winner;</t>
+  </si>
+  <si>
+    <t>car crossed fl in false direction and then crossed in the right direction</t>
+  </si>
+  <si>
+    <t>there is a car on current car path &gt; crashed</t>
+  </si>
+  <si>
+    <t>there is a wall on current car path &gt; crashed</t>
+  </si>
+  <si>
+    <t>there is a fl on current car path &gt; winner if direction ok and pp =0</t>
   </si>
 </sst>
 </file>
@@ -593,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF32F72-142A-4A55-A3DA-B7452AF59065}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -605,9 +679,9 @@
     <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -752,24 +826,76 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="E19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="E19" t="s">
-        <v>25</v>
+      <c r="F19" t="s">
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -782,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -819,10 +945,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -836,13 +962,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -850,19 +976,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -870,19 +996,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -890,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -899,10 +1025,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -910,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -919,10 +1045,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -930,7 +1056,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -939,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -950,7 +1076,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -959,16 +1085,19 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
       <c r="G10">
         <v>90</v>
       </c>
@@ -977,6 +1106,9 @@
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
       <c r="G11">
         <v>180</v>
       </c>
@@ -985,21 +1117,24 @@
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
       <c r="G12">
         <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#37 add test case: doCarTurn_CrossLineInFalseDirectionGoReverseNoWinner(), fix bugs
</commit_message>
<xml_diff>
--- a/documentations/TestsDocumentation.xlsx
+++ b/documentations/TestsDocumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\Studium\ZHAW\Module\02_Semester\PM2\workspaces\intellij_workspace_pm2\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C113089D-3793-4A4D-87C3-1062021484E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04348468-A17D-4D49-A293-CF114C3701D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Expected result</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>if car crashed the cat status is updated und car crash postion is set</t>
+  </si>
+  <si>
+    <t>car croses fl in right direction</t>
+  </si>
+  <si>
+    <t>one stop at start, next collide &gt; last is crashed</t>
   </si>
 </sst>
 </file>
@@ -673,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF32F72-142A-4A55-A3DA-B7452AF59065}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="68" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="68" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -897,6 +903,16 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68531675-09C4-4F5D-A891-F3DADCBB6515}">
   <dimension ref="A3:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#26 add test cases
</commit_message>
<xml_diff>
--- a/documentations/TestsDocumentation.xlsx
+++ b/documentations/TestsDocumentation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\Studium\ZHAW\Module\02_Semester\PM2\workspaces\intellij_workspace_pm2\documentations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47567E4-C541-4044-936F-CAC7C58A9B44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30140" yWindow="0" windowWidth="27580" windowHeight="21740" activeTab="5"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="3" r:id="rId1"/>
@@ -18,18 +24,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
   <si>
     <t>Expected result</t>
   </si>
@@ -255,9 +261,6 @@
     <t>car finishes line in correct direction is  winner</t>
   </si>
   <si>
-    <t>all car crashes one is the winner</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Car </t>
     </r>
@@ -308,9 +311,6 @@
     <t>acceleration = Direction.UP, carIndex = FIRST_TURN_CAR_INDEX</t>
   </si>
   <si>
-    <t>Config.MAX cars total; All cars except one car are crashed ; the last remaining is the winner;</t>
-  </si>
-  <si>
     <t>Two cars, crash one, the last is winner;</t>
   </si>
   <si>
@@ -399,12 +399,21 @@
   </si>
   <si>
     <t>testMap Array</t>
+  </si>
+  <si>
+    <t>Config.MAX cars total;all except one car are crash ; the last remaining car is the winner;</t>
+  </si>
+  <si>
+    <t>car croses fl in right direction</t>
+  </si>
+  <si>
+    <t>one stop at start, next collide &gt; last is crashed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -791,32 +800,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -836,7 +845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -844,7 +853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>1</v>
       </c>
@@ -861,7 +870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>2</v>
       </c>
@@ -878,7 +887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>3</v>
       </c>
@@ -895,7 +904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>4</v>
       </c>
@@ -912,7 +921,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>5</v>
       </c>
@@ -929,7 +938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>6</v>
       </c>
@@ -937,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>7</v>
       </c>
@@ -945,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -953,7 +962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>1</v>
       </c>
@@ -961,16 +970,16 @@
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>20</v>
       </c>
@@ -984,50 +993,55 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F20" t="s">
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="G22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="G26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="G27" t="s">
-        <v>54</v>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1042,25 +1056,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1080,7 +1094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1088,7 +1102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1108,7 +1122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1128,7 +1142,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1148,7 +1162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1168,7 +1182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>5</v>
       </c>
@@ -1188,7 +1202,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>6</v>
       </c>
@@ -1208,7 +1222,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>7</v>
       </c>
@@ -1228,7 +1242,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>8</v>
       </c>
@@ -1239,7 +1253,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>9</v>
       </c>
@@ -1250,7 +1264,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>10</v>
       </c>
@@ -1261,12 +1275,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1285,12 +1299,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1302,12 +1318,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1319,12 +1335,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1336,25 +1352,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="38.1640625" customWidth="1"/>
+    <col min="7" max="7" width="38.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1374,80 +1390,80 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1459,55 +1475,55 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1519,67 +1535,67 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1594,12 +1610,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1611,12 +1627,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>